<commit_message>
new -- youtube 应用MMoE 简单完成
</commit_message>
<xml_diff>
--- a/博客-文章/石晓文/目录--石晓文.xlsx
+++ b/博客-文章/石晓文/目录--石晓文.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\reference\note\博客-文章\石晓文\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3341FEDC-2EC6-44E2-8B6F-34CE7A83B5EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF7CB11-9AC2-44A7-923B-46565ECE130C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="1275" windowWidth="14910" windowHeight="9840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7290" yWindow="1080" windowWidth="13200" windowHeight="9840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="目录" sheetId="1" r:id="rId1"/>
@@ -684,7 +684,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -856,6 +856,14 @@
       <color rgb="FFFF0000"/>
       <name val="等线"/>
       <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="8"/>
+      <name val="等线"/>
+      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1291,7 +1299,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1317,6 +1325,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1677,10 +1691,10 @@
   <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B83" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A69" sqref="A69:A97"/>
+      <selection pane="bottomRight" activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3348,7 +3362,7 @@
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="A69" s="3" t="s">
         <v>113</v>
       </c>
       <c r="C69" t="s">
@@ -3371,7 +3385,7 @@
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="A70" s="9" t="s">
         <v>200</v>
       </c>
       <c r="C70" t="s">
@@ -3442,7 +3456,7 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
+      <c r="A73" s="10" t="s">
         <v>120</v>
       </c>
       <c r="B73" s="2"/>
@@ -3912,7 +3926,7 @@
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
+      <c r="A93" s="10" t="s">
         <v>181</v>
       </c>
       <c r="B93" s="2"/>

</xml_diff>

<commit_message>
new -- PLE 完成
</commit_message>
<xml_diff>
--- a/博客-文章/石晓文/目录--石晓文.xlsx
+++ b/博客-文章/石晓文/目录--石晓文.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\reference\note\博客-文章\石晓文\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF7CB11-9AC2-44A7-923B-46565ECE130C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD322AA6-50F7-43AE-8738-B44E4A566A1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7290" yWindow="1080" windowWidth="13200" windowHeight="9840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1299,7 +1299,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1325,9 +1325,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1">
@@ -1691,10 +1688,10 @@
   <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B92" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A70" sqref="A70"/>
+      <selection pane="bottomRight" activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3385,7 +3382,7 @@
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="9" t="s">
+      <c r="A70" s="3" t="s">
         <v>200</v>
       </c>
       <c r="C70" t="s">
@@ -3456,7 +3453,7 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="10" t="s">
+      <c r="A73" s="5" t="s">
         <v>120</v>
       </c>
       <c r="B73" s="2"/>
@@ -3926,7 +3923,7 @@
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="10" t="s">
+      <c r="A93" s="9" t="s">
         <v>181</v>
       </c>
       <c r="B93" s="2"/>

</xml_diff>